<commit_message>
Ajuste busca de e-mail, criação de arquivo .xlsx com o resultado das buscas
</commit_message>
<xml_diff>
--- a/Arquivos/base test.xlsx
+++ b/Arquivos/base test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projeto leitor de e-mail\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projeto leitor de e-mail\Arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36001241-DB9B-4DB3-B4A3-4004EE6B0204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6161EF04-AB9D-4160-B369-5EFB89E3C327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C9D92BB9-386A-47C4-A3F0-57D6F0E7D085}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="17">
   <si>
     <t>Voucher</t>
   </si>
@@ -138,9 +138,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,9 +478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4D44A8E-6317-4C1F-98E8-833D2286B507}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -488,7 +487,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -496,23 +495,23 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1234</v>
+      <c r="A2" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>12345</v>
+      <c r="A3" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
@@ -520,7 +519,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
@@ -528,7 +527,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
@@ -536,7 +535,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B7" t="s">

</xml_diff>